<commit_message>
Correction suite à validation ECF
</commit_message>
<xml_diff>
--- a/LKU - Etape1/Dictionnaire des données & Règles.xlsx
+++ b/LKU - Etape1/Dictionnaire des données & Règles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Nom donnée</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Type</t>
   </si>
   <si>
+    <t>Obligatoire</t>
+  </si>
+  <si>
     <t>nomPays</t>
   </si>
   <si>
@@ -32,6 +35,9 @@
   </si>
   <si>
     <t>Chaîne de caractères</t>
+  </si>
+  <si>
+    <t>Oui</t>
   </si>
   <si>
     <t>nomRegion</t>
@@ -525,7 +531,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -551,299 +559,380 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -872,10 +961,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -908,7 +997,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
@@ -917,7 +1006,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -926,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -935,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
@@ -944,7 +1033,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
@@ -953,7 +1042,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
@@ -962,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
@@ -971,7 +1060,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
@@ -980,7 +1069,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11">
@@ -989,7 +1078,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12">
@@ -998,7 +1087,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13">
@@ -1007,7 +1096,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
@@ -1016,7 +1105,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -1025,7 +1114,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
@@ -1034,7 +1123,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
@@ -1043,7 +1132,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
@@ -1052,7 +1141,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19">
@@ -1061,7 +1150,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20">
@@ -1070,7 +1159,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21">
@@ -1079,7 +1168,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>